<commit_message>
Fixed pin numbers in connections to match up with gvanhoy's assignments
</commit_message>
<xml_diff>
--- a/Connections_Tables.xlsx
+++ b/Connections_Tables.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="51">
   <si>
     <t>Expansion Board J11</t>
   </si>
@@ -133,9 +133,6 @@
     <t>LCD (4)</t>
   </si>
   <si>
-    <t>LCD (5)</t>
-  </si>
-  <si>
     <t>Expansion Board J11 (22)</t>
   </si>
   <si>
@@ -148,36 +145,9 @@
     <t>Expansion Board J10</t>
   </si>
   <si>
-    <t>Expansion Board J10 (1)</t>
-  </si>
-  <si>
     <t>Expansion Board J10 (5)</t>
   </si>
   <si>
-    <t>LCD (7)</t>
-  </si>
-  <si>
-    <t>LCD (8)</t>
-  </si>
-  <si>
-    <t>LCD (9)</t>
-  </si>
-  <si>
-    <t>LCD(10)</t>
-  </si>
-  <si>
-    <t>LCD(14)</t>
-  </si>
-  <si>
-    <t>LCD(11)</t>
-  </si>
-  <si>
-    <t>LCD(12)</t>
-  </si>
-  <si>
-    <t>LCD(13)</t>
-  </si>
-  <si>
     <t>Expansion Board J10 (7)</t>
   </si>
   <si>
@@ -187,25 +157,28 @@
     <t>Expansion Board J10 (11)</t>
   </si>
   <si>
-    <t>Expansion Board J10 (13)</t>
-  </si>
-  <si>
-    <t>Expansion Board J10 (15)</t>
-  </si>
-  <si>
-    <t>Expansion Board J10 (17)</t>
-  </si>
-  <si>
     <t>Expansion Board J10 (19)</t>
   </si>
   <si>
     <t>Expansion Board J10 (21)</t>
   </si>
   <si>
-    <t>Expansion Board J10 (29)</t>
-  </si>
-  <si>
     <t>`</t>
+  </si>
+  <si>
+    <t>LCD (11)</t>
+  </si>
+  <si>
+    <t>LCD (12)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Blue </t>
+  </si>
+  <si>
+    <t>LCD (13)</t>
+  </si>
+  <si>
+    <t>LCD (14)</t>
   </si>
 </sst>
 </file>
@@ -738,7 +711,7 @@
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5">
-        <f t="shared" ref="A5:A21" si="0" xml:space="preserve"> A4+2</f>
+        <f t="shared" ref="A5:A20" si="0" xml:space="preserve"> A4+2</f>
         <v>6</v>
       </c>
       <c r="B5" t="s">
@@ -1042,7 +1015,7 @@
   <dimension ref="A1:K28"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="S27" sqref="S27"/>
+      <selection activeCell="K28" sqref="K28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1063,7 +1036,7 @@
         <v>0</v>
       </c>
       <c r="E1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I1" t="s">
         <v>28</v>
@@ -1111,20 +1084,15 @@
       <c r="E3">
         <v>1</v>
       </c>
-      <c r="F3" t="s">
-        <v>38</v>
-      </c>
-      <c r="G3" s="7" t="s">
-        <v>25</v>
-      </c>
+      <c r="G3" s="6"/>
       <c r="I3">
         <v>1</v>
       </c>
       <c r="J3" t="s">
+        <v>35</v>
+      </c>
+      <c r="K3" s="9" t="s">
         <v>36</v>
-      </c>
-      <c r="K3" s="9" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -1170,14 +1138,14 @@
         <v>3</v>
       </c>
       <c r="E5">
-        <f t="shared" ref="E5:E25" si="1">E4+2</f>
+        <f t="shared" ref="E5:E21" si="1">E4+2</f>
         <v>5</v>
       </c>
       <c r="F5" t="s">
-        <v>34</v>
-      </c>
-      <c r="G5" s="7" t="s">
-        <v>25</v>
+        <v>46</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>6</v>
       </c>
       <c r="I5">
         <v>3</v>
@@ -1205,16 +1173,16 @@
         <v>7</v>
       </c>
       <c r="F6" t="s">
-        <v>35</v>
-      </c>
-      <c r="G6" s="7" t="s">
-        <v>25</v>
+        <v>47</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>6</v>
       </c>
       <c r="I6">
         <v>4</v>
       </c>
       <c r="J6" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="K6" s="7" t="s">
         <v>25</v>
@@ -1236,7 +1204,7 @@
         <v>9</v>
       </c>
       <c r="F7" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="G7" s="8" t="s">
         <v>6</v>
@@ -1245,10 +1213,10 @@
         <v>5</v>
       </c>
       <c r="J7" t="s">
-        <v>50</v>
-      </c>
-      <c r="K7" s="7" t="s">
-        <v>25</v>
+        <v>3</v>
+      </c>
+      <c r="K7" s="6" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -1267,7 +1235,7 @@
         <v>11</v>
       </c>
       <c r="F8" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="G8" s="8" t="s">
         <v>6</v>
@@ -1276,7 +1244,7 @@
         <v>6</v>
       </c>
       <c r="J8" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="K8" s="7" t="s">
         <v>25</v>
@@ -1298,19 +1266,19 @@
         <v>13</v>
       </c>
       <c r="F9" t="s">
-        <v>44</v>
-      </c>
-      <c r="G9" s="8" t="s">
-        <v>6</v>
+        <v>3</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>3</v>
       </c>
       <c r="I9">
         <v>7</v>
       </c>
       <c r="J9" t="s">
-        <v>51</v>
-      </c>
-      <c r="K9" s="8" t="s">
-        <v>6</v>
+        <v>3</v>
+      </c>
+      <c r="K9" s="6" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -1329,19 +1297,19 @@
         <v>15</v>
       </c>
       <c r="F10" t="s">
-        <v>45</v>
-      </c>
-      <c r="G10" s="8" t="s">
-        <v>6</v>
+        <v>3</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>3</v>
       </c>
       <c r="I10">
         <v>8</v>
       </c>
       <c r="J10" t="s">
-        <v>52</v>
-      </c>
-      <c r="K10" s="8" t="s">
-        <v>6</v>
+        <v>3</v>
+      </c>
+      <c r="K10" s="6" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
@@ -1360,19 +1328,19 @@
         <v>17</v>
       </c>
       <c r="F11" t="s">
-        <v>47</v>
-      </c>
-      <c r="G11" s="8" t="s">
-        <v>6</v>
+        <v>3</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>3</v>
       </c>
       <c r="I11">
         <v>9</v>
       </c>
       <c r="J11" t="s">
-        <v>53</v>
-      </c>
-      <c r="K11" s="8" t="s">
-        <v>6</v>
+        <v>3</v>
+      </c>
+      <c r="K11" s="6" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
@@ -1384,26 +1352,26 @@
         <v>33</v>
       </c>
       <c r="C12" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="1"/>
+        <v>19</v>
+      </c>
+      <c r="F12" t="s">
         <v>37</v>
       </c>
-      <c r="E12">
-        <f t="shared" si="1"/>
-        <v>19</v>
-      </c>
-      <c r="F12" t="s">
-        <v>48</v>
-      </c>
-      <c r="G12" s="8" t="s">
-        <v>6</v>
+      <c r="G12" s="7" t="s">
+        <v>25</v>
       </c>
       <c r="I12">
         <v>10</v>
       </c>
       <c r="J12" t="s">
-        <v>54</v>
-      </c>
-      <c r="K12" s="8" t="s">
-        <v>6</v>
+        <v>3</v>
+      </c>
+      <c r="K12" s="6" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -1422,16 +1390,16 @@
         <v>21</v>
       </c>
       <c r="F13" t="s">
-        <v>49</v>
-      </c>
-      <c r="G13" s="8" t="s">
-        <v>6</v>
+        <v>34</v>
+      </c>
+      <c r="G13" s="7" t="s">
+        <v>25</v>
       </c>
       <c r="I13">
         <v>11</v>
       </c>
       <c r="J13" t="s">
-        <v>55</v>
+        <v>39</v>
       </c>
       <c r="K13" s="8" t="s">
         <v>6</v>
@@ -1462,10 +1430,10 @@
         <v>12</v>
       </c>
       <c r="J14" t="s">
-        <v>56</v>
+        <v>40</v>
       </c>
       <c r="K14" s="8" t="s">
-        <v>6</v>
+        <v>48</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
@@ -1493,7 +1461,7 @@
         <v>13</v>
       </c>
       <c r="J15" t="s">
-        <v>57</v>
+        <v>41</v>
       </c>
       <c r="K15" s="8" t="s">
         <v>6</v>
@@ -1524,7 +1492,7 @@
         <v>14</v>
       </c>
       <c r="J16" t="s">
-        <v>58</v>
+        <v>42</v>
       </c>
       <c r="K16" s="8" t="s">
         <v>6</v>
@@ -1546,10 +1514,10 @@
         <v>29</v>
       </c>
       <c r="F17" t="s">
-        <v>46</v>
-      </c>
-      <c r="G17" s="8" t="s">
-        <v>6</v>
+        <v>3</v>
+      </c>
+      <c r="G17" s="6" t="s">
+        <v>3</v>
       </c>
       <c r="I17">
         <v>15</v>
@@ -1714,7 +1682,7 @@
         <v>3</v>
       </c>
       <c r="E24">
-        <f t="shared" ref="E24:E30" si="2">E23+2</f>
+        <f t="shared" ref="E24:E28" si="2">E23+2</f>
         <v>51</v>
       </c>
       <c r="F24" t="s">
@@ -1792,8 +1760,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E41" sqref="E41"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N29" sqref="N29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1821,7 +1789,7 @@
         <v>0</v>
       </c>
       <c r="E1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I1" t="s">
         <v>28</v>
@@ -1881,20 +1849,15 @@
       <c r="E3">
         <v>1</v>
       </c>
-      <c r="F3" t="s">
-        <v>38</v>
-      </c>
-      <c r="G3" s="7" t="s">
-        <v>25</v>
-      </c>
+      <c r="G3" s="6"/>
       <c r="I3">
         <v>1</v>
       </c>
       <c r="J3" t="s">
+        <v>35</v>
+      </c>
+      <c r="K3" s="9" t="s">
         <v>36</v>
-      </c>
-      <c r="K3" s="9" t="s">
-        <v>37</v>
       </c>
       <c r="M3">
         <v>1</v>
@@ -1948,7 +1911,7 @@
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5">
-        <f t="shared" ref="A5:A21" si="0" xml:space="preserve"> A4+2</f>
+        <f t="shared" ref="A5:A20" si="0" xml:space="preserve"> A4+2</f>
         <v>6</v>
       </c>
       <c r="B5" t="s">
@@ -1958,14 +1921,14 @@
         <v>3</v>
       </c>
       <c r="E5">
-        <f t="shared" ref="E5:E25" si="1">E4+2</f>
+        <f t="shared" ref="E5:E21" si="1">E4+2</f>
         <v>5</v>
       </c>
       <c r="F5" t="s">
-        <v>34</v>
-      </c>
-      <c r="G5" s="7" t="s">
-        <v>25</v>
+        <v>46</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>6</v>
       </c>
       <c r="I5">
         <v>3</v>
@@ -2002,16 +1965,16 @@
         <v>7</v>
       </c>
       <c r="F6" t="s">
-        <v>35</v>
-      </c>
-      <c r="G6" s="7" t="s">
-        <v>25</v>
+        <v>47</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>6</v>
       </c>
       <c r="I6">
         <v>4</v>
       </c>
       <c r="J6" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="K6" s="7" t="s">
         <v>25</v>
@@ -2042,7 +2005,7 @@
         <v>9</v>
       </c>
       <c r="F7" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="G7" s="8" t="s">
         <v>6</v>
@@ -2051,10 +2014,10 @@
         <v>5</v>
       </c>
       <c r="J7" t="s">
-        <v>50</v>
-      </c>
-      <c r="K7" s="7" t="s">
-        <v>25</v>
+        <v>3</v>
+      </c>
+      <c r="K7" s="6" t="s">
+        <v>3</v>
       </c>
       <c r="M7">
         <v>5</v>
@@ -2082,7 +2045,7 @@
         <v>11</v>
       </c>
       <c r="F8" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="G8" s="8" t="s">
         <v>6</v>
@@ -2091,7 +2054,7 @@
         <v>6</v>
       </c>
       <c r="J8" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="K8" s="7" t="s">
         <v>25</v>
@@ -2122,19 +2085,19 @@
         <v>13</v>
       </c>
       <c r="F9" t="s">
-        <v>44</v>
-      </c>
-      <c r="G9" s="8" t="s">
-        <v>6</v>
+        <v>3</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>3</v>
       </c>
       <c r="I9">
         <v>7</v>
       </c>
       <c r="J9" t="s">
-        <v>51</v>
-      </c>
-      <c r="K9" s="8" t="s">
-        <v>6</v>
+        <v>3</v>
+      </c>
+      <c r="K9" s="6" t="s">
+        <v>3</v>
       </c>
       <c r="M9">
         <v>7</v>
@@ -2162,19 +2125,19 @@
         <v>15</v>
       </c>
       <c r="F10" t="s">
-        <v>45</v>
-      </c>
-      <c r="G10" s="8" t="s">
-        <v>6</v>
+        <v>3</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>3</v>
       </c>
       <c r="I10">
         <v>8</v>
       </c>
       <c r="J10" t="s">
-        <v>52</v>
-      </c>
-      <c r="K10" s="8" t="s">
-        <v>6</v>
+        <v>3</v>
+      </c>
+      <c r="K10" s="6" t="s">
+        <v>3</v>
       </c>
       <c r="M10">
         <v>8</v>
@@ -2202,19 +2165,19 @@
         <v>17</v>
       </c>
       <c r="F11" t="s">
-        <v>47</v>
-      </c>
-      <c r="G11" s="8" t="s">
-        <v>6</v>
+        <v>3</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>3</v>
       </c>
       <c r="I11">
         <v>9</v>
       </c>
       <c r="J11" t="s">
-        <v>53</v>
-      </c>
-      <c r="K11" s="8" t="s">
-        <v>6</v>
+        <v>3</v>
+      </c>
+      <c r="K11" s="6" t="s">
+        <v>3</v>
       </c>
       <c r="M11">
         <v>9</v>
@@ -2242,19 +2205,19 @@
         <v>19</v>
       </c>
       <c r="F12" t="s">
-        <v>48</v>
-      </c>
-      <c r="G12" s="8" t="s">
-        <v>6</v>
+        <v>37</v>
+      </c>
+      <c r="G12" s="7" t="s">
+        <v>25</v>
       </c>
       <c r="I12">
         <v>10</v>
       </c>
       <c r="J12" t="s">
-        <v>54</v>
-      </c>
-      <c r="K12" s="8" t="s">
-        <v>6</v>
+        <v>3</v>
+      </c>
+      <c r="K12" s="6" t="s">
+        <v>3</v>
       </c>
       <c r="M12">
         <v>10</v>
@@ -2275,23 +2238,23 @@
         <v>33</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E13">
         <f t="shared" si="1"/>
         <v>21</v>
       </c>
       <c r="F13" t="s">
-        <v>49</v>
-      </c>
-      <c r="G13" s="8" t="s">
-        <v>6</v>
+        <v>34</v>
+      </c>
+      <c r="G13" s="7" t="s">
+        <v>25</v>
       </c>
       <c r="I13">
         <v>11</v>
       </c>
       <c r="J13" t="s">
-        <v>55</v>
+        <v>39</v>
       </c>
       <c r="K13" s="8" t="s">
         <v>6</v>
@@ -2322,10 +2285,10 @@
         <v>12</v>
       </c>
       <c r="J14" t="s">
-        <v>56</v>
+        <v>40</v>
       </c>
       <c r="K14" s="8" t="s">
-        <v>6</v>
+        <v>48</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
@@ -2353,7 +2316,7 @@
         <v>13</v>
       </c>
       <c r="J15" t="s">
-        <v>57</v>
+        <v>41</v>
       </c>
       <c r="K15" s="8" t="s">
         <v>6</v>
@@ -2384,7 +2347,7 @@
         <v>14</v>
       </c>
       <c r="J16" t="s">
-        <v>58</v>
+        <v>42</v>
       </c>
       <c r="K16" s="8" t="s">
         <v>6</v>
@@ -2406,10 +2369,10 @@
         <v>29</v>
       </c>
       <c r="F17" t="s">
-        <v>46</v>
-      </c>
-      <c r="G17" s="8" t="s">
-        <v>6</v>
+        <v>3</v>
+      </c>
+      <c r="G17" s="6" t="s">
+        <v>3</v>
       </c>
       <c r="I17">
         <v>15</v>
@@ -2507,7 +2470,7 @@
         <v>31</v>
       </c>
       <c r="D21" t="s">
-        <v>59</v>
+        <v>45</v>
       </c>
       <c r="E21">
         <f t="shared" si="1"/>
@@ -2697,5 +2660,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>